<commit_message>
Third commit - after issue resolved
</commit_message>
<xml_diff>
--- a/Luma/target/test-classes/TestData.xlsx
+++ b/Luma/target/test-classes/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sathishkumar.a\Desktop\sathish\Projects\Luma\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sathishkumar.a\Desktop\sathish\Projects\Git repositories\Luma\Luma\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D293CD10-C04D-4DA3-92D3-EE6767D19AF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D46BCC-2639-4F6D-A683-F4DFCA915CB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14240" windowHeight="4070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Logoipsum" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Yes</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>SignIn</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
 </sst>
 </file>
@@ -429,7 +426,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A4" sqref="A4:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -475,7 +472,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>

</xml_diff>